<commit_message>
Added function to fill CHAIRS-Table to map lectures to subjects.
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Source/University/university-app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Source/TUM/university-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A764B6FE-FFF8-5446-921B-A0E9315C2234}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060ED99C-8040-1B45-9964-D5837F56B217}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="460" windowWidth="25000" windowHeight="14980" xr2:uid="{116BA031-35A0-0A47-8133-2278F0BBD56B}"/>
+    <workbookView xWindow="300" yWindow="460" windowWidth="25000" windowHeight="14980" activeTab="2" xr2:uid="{116BA031-35A0-0A47-8133-2278F0BBD56B}"/>
   </bookViews>
   <sheets>
     <sheet name="STUDENTS" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CHAIRS" sheetId="5" r:id="rId3"/>
     <sheet name="ATTENDS" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>Prof. Mayer</t>
+  </si>
+  <si>
+    <t>SUBJECT</t>
   </si>
 </sst>
 </file>
@@ -628,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF524D4F-E762-414B-B490-FB47FC0916C2}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2757,8 +2760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA7B982-A8FB-2B42-9B70-CF2E4E4052FE}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2775,7 +2778,7 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3">

</xml_diff>

<commit_message>
Change "place" in schema to "roomnumber" and "buildingnumber"
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Source/TUM/university-app/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnd\Documents\second semester in TUM\pom\universityapp0522\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060ED99C-8040-1B45-9964-D5837F56B217}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FBEB8558-D583-4864-A333-44E9E265B333}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="460" windowWidth="25000" windowHeight="14980" activeTab="2" xr2:uid="{116BA031-35A0-0A47-8133-2278F0BBD56B}"/>
+    <workbookView xWindow="300" yWindow="458" windowWidth="24998" windowHeight="14978" activeTab="1" xr2:uid="{116BA031-35A0-0A47-8133-2278F0BBD56B}"/>
   </bookViews>
   <sheets>
     <sheet name="STUDENTS" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CHAIRS" sheetId="5" r:id="rId3"/>
     <sheet name="ATTENDS" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -57,9 +57,6 @@
     <t>TIME</t>
   </si>
   <si>
-    <t>PLACE</t>
-  </si>
-  <si>
     <t>LECTURER</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>Mo., 11:30-13:00</t>
   </si>
   <si>
-    <t>MI01</t>
-  </si>
-  <si>
     <t>Planning and Scheduling of Complex Operations: Models, Methods and Applications</t>
   </si>
   <si>
@@ -189,9 +183,6 @@
     <t>Di., 8:00-14:00</t>
   </si>
   <si>
-    <t>WI01</t>
-  </si>
-  <si>
     <t>Höhere Mathematik 1</t>
   </si>
   <si>
@@ -237,9 +228,6 @@
     <t>Do., 9:00-11:30</t>
   </si>
   <si>
-    <t>ME01</t>
-  </si>
-  <si>
     <t xml:space="preserve">Prof. Moritz </t>
   </si>
   <si>
@@ -268,6 +256,12 @@
   </si>
   <si>
     <t>SUBJECT</t>
+  </si>
+  <si>
+    <t>ROOMNUMBER</t>
+  </si>
+  <si>
+    <t>BUILDINGNUMBER</t>
   </si>
 </sst>
 </file>
@@ -317,7 +311,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -333,7 +327,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -635,12 +629,12 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.71875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="1"/>
+    <col min="2" max="2" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.27734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.71875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -662,13 +656,13 @@
         <v>3953</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -676,13 +670,13 @@
         <v>9764</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -690,13 +684,13 @@
         <v>8064</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -704,13 +698,13 @@
         <v>7355</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -718,13 +712,13 @@
         <v>971</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -800,25 +794,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D067B7-36CB-5347-9E1C-FA227B65D6E2}">
-  <dimension ref="A1:I233"/>
+  <dimension ref="A1:J233"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.71875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1"/>
-    <col min="2" max="2" width="67.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" style="1"/>
-    <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="1"/>
-    <col min="8" max="8" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="1" width="10.71875" style="1"/>
+    <col min="2" max="2" width="67.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.71875" style="1"/>
+    <col min="6" max="6" width="14.27734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.27734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.71875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -838,24 +833,27 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="5">
         <v>5</v>
@@ -864,28 +862,31 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="4" t="str">
+        <v>37</v>
+      </c>
+      <c r="G2" s="4">
+        <v>102</v>
+      </c>
+      <c r="H2" s="4">
+        <v>5620</v>
+      </c>
+      <c r="I2" s="4" t="str">
         <f>VLOOKUP(C2,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Mustermann</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="5">
         <v>6</v>
@@ -894,28 +895,31 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="4" t="str">
+        <v>37</v>
+      </c>
+      <c r="G3" s="4">
+        <v>102</v>
+      </c>
+      <c r="H3" s="4">
+        <v>5620</v>
+      </c>
+      <c r="I3" s="4" t="str">
         <f>VLOOKUP(C3,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Mustermann</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="5">
         <v>6</v>
@@ -924,28 +928,31 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="4" t="str">
+        <v>37</v>
+      </c>
+      <c r="G4" s="4">
+        <v>102</v>
+      </c>
+      <c r="H4" s="4">
+        <v>5620</v>
+      </c>
+      <c r="I4" s="4" t="str">
         <f>VLOOKUP(C4,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Mustermann</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="5">
         <v>5</v>
@@ -954,28 +961,31 @@
         <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="4" t="str">
+        <v>37</v>
+      </c>
+      <c r="G5" s="4">
+        <v>102</v>
+      </c>
+      <c r="H5" s="4">
+        <v>5620</v>
+      </c>
+      <c r="I5" s="4" t="str">
         <f>VLOOKUP(C5,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Müller</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="5">
         <v>8</v>
@@ -984,28 +994,31 @@
         <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="4" t="str">
+        <v>37</v>
+      </c>
+      <c r="G6" s="4">
+        <v>102</v>
+      </c>
+      <c r="H6" s="4">
+        <v>5620</v>
+      </c>
+      <c r="I6" s="4" t="str">
         <f>VLOOKUP(C6,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Schmidt</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="5">
         <v>6</v>
@@ -1014,28 +1027,31 @@
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="4" t="str">
+        <v>37</v>
+      </c>
+      <c r="G7" s="4">
+        <v>102</v>
+      </c>
+      <c r="H7" s="4">
+        <v>5620</v>
+      </c>
+      <c r="I7" s="4" t="str">
         <f>VLOOKUP(C7,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Müller</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="5">
         <v>6</v>
@@ -1044,28 +1060,31 @@
         <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="4" t="str">
+        <v>37</v>
+      </c>
+      <c r="G8" s="4">
+        <v>102</v>
+      </c>
+      <c r="H8" s="4">
+        <v>5620</v>
+      </c>
+      <c r="I8" s="4" t="str">
         <f>VLOOKUP(C8,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Schmidt</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="5">
         <v>6</v>
@@ -1074,28 +1093,31 @@
         <v>3</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="4" t="str">
+        <v>37</v>
+      </c>
+      <c r="G9" s="4">
+        <v>102</v>
+      </c>
+      <c r="H9" s="4">
+        <v>5620</v>
+      </c>
+      <c r="I9" s="4" t="str">
         <f>VLOOKUP(C9,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Mustermann</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="5">
         <v>6</v>
@@ -1104,28 +1126,31 @@
         <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="4" t="str">
+        <v>37</v>
+      </c>
+      <c r="G10" s="4">
+        <v>102</v>
+      </c>
+      <c r="H10" s="4">
+        <v>5620</v>
+      </c>
+      <c r="I10" s="4" t="str">
         <f>VLOOKUP(C10,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Schmidt</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="5">
         <v>5</v>
@@ -1134,28 +1159,31 @@
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="4" t="str">
+        <v>37</v>
+      </c>
+      <c r="G11" s="4">
+        <v>102</v>
+      </c>
+      <c r="H11" s="4">
+        <v>5620</v>
+      </c>
+      <c r="I11" s="4" t="str">
         <f>VLOOKUP(C11,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Müller</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="5">
         <v>6</v>
@@ -1164,28 +1192,31 @@
         <v>4</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="4" t="str">
+        <v>37</v>
+      </c>
+      <c r="G12" s="4">
+        <v>102</v>
+      </c>
+      <c r="H12" s="4">
+        <v>5620</v>
+      </c>
+      <c r="I12" s="4" t="str">
         <f>VLOOKUP(C12,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Mustermann</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="5">
         <v>5</v>
@@ -1194,28 +1225,31 @@
         <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="4" t="str">
+        <v>37</v>
+      </c>
+      <c r="G13" s="4">
+        <v>102</v>
+      </c>
+      <c r="H13" s="4">
+        <v>5620</v>
+      </c>
+      <c r="I13" s="4" t="str">
         <f>VLOOKUP(C13,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Schmidt</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D14" s="4">
         <v>6</v>
@@ -1224,28 +1258,31 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="4" t="str">
+        <v>50</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1801</v>
+      </c>
+      <c r="H14" s="4">
+        <v>5508</v>
+      </c>
+      <c r="I14" s="4" t="str">
         <f>VLOOKUP(C14,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Heinz</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D15" s="4">
         <v>6</v>
@@ -1254,28 +1291,31 @@
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="4" t="str">
+        <v>50</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1801</v>
+      </c>
+      <c r="H15" s="4">
+        <v>5508</v>
+      </c>
+      <c r="I15" s="4" t="str">
         <f>VLOOKUP(C15,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v xml:space="preserve">Prof. Moritz </v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16" s="4">
         <v>6</v>
@@ -1284,28 +1324,31 @@
         <v>2</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="4" t="str">
+        <v>50</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1801</v>
+      </c>
+      <c r="H16" s="4">
+        <v>5508</v>
+      </c>
+      <c r="I16" s="4" t="str">
         <f>VLOOKUP(C16,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Peter</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17" s="4">
         <v>6</v>
@@ -1314,28 +1357,31 @@
         <v>2</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="4" t="str">
+        <v>50</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1801</v>
+      </c>
+      <c r="H17" s="4">
+        <v>5508</v>
+      </c>
+      <c r="I17" s="4" t="str">
         <f>VLOOKUP(C17,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v xml:space="preserve">Prof. Moritz </v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" s="4">
         <v>6</v>
@@ -1344,28 +1390,31 @@
         <v>3</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="4" t="str">
+        <v>50</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1801</v>
+      </c>
+      <c r="H18" s="4">
+        <v>5508</v>
+      </c>
+      <c r="I18" s="4" t="str">
         <f>VLOOKUP(C18,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Peter</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D19" s="4">
         <v>6</v>
@@ -1374,28 +1423,31 @@
         <v>3</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="4" t="str">
+        <v>50</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1801</v>
+      </c>
+      <c r="H19" s="4">
+        <v>5508</v>
+      </c>
+      <c r="I19" s="4" t="str">
         <f>VLOOKUP(C19,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v xml:space="preserve">Prof. Moritz </v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D20" s="4">
         <v>6</v>
@@ -1404,28 +1456,31 @@
         <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="4" t="str">
+        <v>50</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1801</v>
+      </c>
+      <c r="H20" s="4">
+        <v>5508</v>
+      </c>
+      <c r="I20" s="4" t="str">
         <f>VLOOKUP(C20,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Heinz</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D21" s="4">
         <v>6</v>
@@ -1434,28 +1489,31 @@
         <v>4</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H21" s="4" t="str">
+        <v>50</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1801</v>
+      </c>
+      <c r="H21" s="4">
+        <v>5508</v>
+      </c>
+      <c r="I21" s="4" t="str">
         <f>VLOOKUP(C21,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Peter</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D22" s="4">
         <v>6</v>
@@ -1464,28 +1522,31 @@
         <v>5</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H22" s="4" t="str">
+        <v>50</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1801</v>
+      </c>
+      <c r="H22" s="4">
+        <v>5508</v>
+      </c>
+      <c r="I22" s="4" t="str">
         <f>VLOOKUP(C22,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Heinz</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D23" s="4">
         <v>8</v>
@@ -1494,28 +1555,31 @@
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H23" s="4" t="str">
+        <v>65</v>
+      </c>
+      <c r="G23" s="4">
+        <v>2501</v>
+      </c>
+      <c r="H23" s="4">
+        <v>5101</v>
+      </c>
+      <c r="I23" s="4" t="str">
         <f>VLOOKUP(C23,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Meier</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D24" s="4">
         <v>8</v>
@@ -1524,28 +1588,31 @@
         <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H24" s="4" t="str">
+        <v>65</v>
+      </c>
+      <c r="G24" s="4">
+        <v>2501</v>
+      </c>
+      <c r="H24" s="4">
+        <v>5101</v>
+      </c>
+      <c r="I24" s="4" t="str">
         <f>VLOOKUP(C24,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Meier</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D25" s="4">
         <v>2</v>
@@ -1554,28 +1621,31 @@
         <v>1</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H25" s="4" t="str">
+        <v>65</v>
+      </c>
+      <c r="G25" s="4">
+        <v>2501</v>
+      </c>
+      <c r="H25" s="4">
+        <v>5101</v>
+      </c>
+      <c r="I25" s="4" t="str">
         <f>VLOOKUP(C25,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Schmidt</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D26" s="4">
         <v>3</v>
@@ -1584,28 +1654,31 @@
         <v>2</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H26" s="4" t="str">
+        <v>65</v>
+      </c>
+      <c r="G26" s="4">
+        <v>2501</v>
+      </c>
+      <c r="H26" s="4">
+        <v>5101</v>
+      </c>
+      <c r="I26" s="4" t="str">
         <f>VLOOKUP(C26,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Schmidt</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D27" s="4">
         <v>3</v>
@@ -1614,28 +1687,31 @@
         <v>3</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H27" s="4" t="str">
+        <v>65</v>
+      </c>
+      <c r="G27" s="4">
+        <v>2501</v>
+      </c>
+      <c r="H27" s="4">
+        <v>5101</v>
+      </c>
+      <c r="I27" s="4" t="str">
         <f>VLOOKUP(C27,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Hermann</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D28" s="4">
         <v>6</v>
@@ -1644,28 +1720,31 @@
         <v>3</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H28" s="4" t="str">
+        <v>65</v>
+      </c>
+      <c r="G28" s="4">
+        <v>2501</v>
+      </c>
+      <c r="H28" s="4">
+        <v>5101</v>
+      </c>
+      <c r="I28" s="4" t="str">
         <f>VLOOKUP(C28,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Hermann</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D29" s="4">
         <v>6</v>
@@ -1674,28 +1753,31 @@
         <v>4</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H29" s="4" t="str">
+        <v>65</v>
+      </c>
+      <c r="G29" s="4">
+        <v>2501</v>
+      </c>
+      <c r="H29" s="4">
+        <v>5101</v>
+      </c>
+      <c r="I29" s="4" t="str">
         <f>VLOOKUP(C29,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Hermann</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D30" s="4">
         <v>8</v>
@@ -1704,28 +1786,31 @@
         <v>4</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H30" s="4" t="str">
+        <v>65</v>
+      </c>
+      <c r="G30" s="4">
+        <v>2501</v>
+      </c>
+      <c r="H30" s="4">
+        <v>5101</v>
+      </c>
+      <c r="I30" s="4" t="str">
         <f>VLOOKUP(C30,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Mayer</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D31" s="4">
         <v>8</v>
@@ -1734,28 +1819,31 @@
         <v>5</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H31" s="4" t="str">
+        <v>65</v>
+      </c>
+      <c r="G31" s="4">
+        <v>2501</v>
+      </c>
+      <c r="H31" s="4">
+        <v>5101</v>
+      </c>
+      <c r="I31" s="4" t="str">
         <f>VLOOKUP(C31,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Mayer</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D32" s="4">
         <v>5</v>
@@ -1764,96 +1852,103 @@
         <v>3</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H32" s="4" t="str">
+        <v>65</v>
+      </c>
+      <c r="G32" s="4">
+        <v>2501</v>
+      </c>
+      <c r="H32" s="4">
+        <v>5101</v>
+      </c>
+      <c r="I32" s="4" t="str">
         <f>VLOOKUP(C32,CHAIRS!$A$2:$B$11,2,FALSE)</f>
         <v>Prof. Mayer</v>
       </c>
-      <c r="I32" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="J32" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="4"/>
       <c r="B33"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:8">
       <c r="A36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:8">
       <c r="A37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:8">
       <c r="A38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:8">
       <c r="A39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:8">
       <c r="A40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:8">
       <c r="A41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:8">
       <c r="A42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:8">
       <c r="A43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:8">
       <c r="A44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:8">
       <c r="A45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:8">
       <c r="A46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:8">
       <c r="A47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:8">
       <c r="A48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -2760,14 +2855,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA7B982-A8FB-2B42-9B70-CF2E4E4052FE}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2775,120 +2870,120 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2904,17 +2999,17 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.71875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="10.7109375" style="4"/>
+    <col min="1" max="16384" width="10.71875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Added comments table to project
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnd\Documents\second semester in TUM\pom\universityapp0522\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\IdeaProjects\University-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FBEB8558-D583-4864-A333-44E9E265B333}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="458" windowWidth="24998" windowHeight="14978" activeTab="1" xr2:uid="{116BA031-35A0-0A47-8133-2278F0BBD56B}"/>
+    <workbookView xWindow="300" yWindow="456" windowWidth="24996" windowHeight="14976" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="STUDENTS" sheetId="1" r:id="rId1"/>
     <sheet name="LECTURES" sheetId="2" r:id="rId2"/>
-    <sheet name="CHAIRS" sheetId="5" r:id="rId3"/>
-    <sheet name="ATTENDS" sheetId="3" r:id="rId4"/>
+    <sheet name="COMMENTS" sheetId="6" r:id="rId3"/>
+    <sheet name="CHAIRS" sheetId="5" r:id="rId4"/>
+    <sheet name="ATTENDS" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -262,12 +262,33 @@
   </si>
   <si>
     <t>BUILDINGNUMBER</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>CONTENT</t>
+  </si>
+  <si>
+    <t>4 out of 7, would recommend</t>
+  </si>
+  <si>
+    <t>Great</t>
+  </si>
+  <si>
+    <t>Could be better organized</t>
+  </si>
+  <si>
+    <t>It's bollocks</t>
+  </si>
+  <si>
+    <t>Nah</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -302,16 +323,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -622,19 +646,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF524D4F-E762-414B-B490-FB47FC0916C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.71875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.27734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.71875" style="1"/>
+    <col min="2" max="2" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -793,24 +817,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D067B7-36CB-5347-9E1C-FA227B65D6E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.71875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.71875" style="1"/>
-    <col min="2" max="2" width="67.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.71875" style="1"/>
-    <col min="6" max="6" width="14.27734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.27734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.71875" style="1"/>
+    <col min="1" max="1" width="10.7265625" style="1"/>
+    <col min="2" max="2" width="67.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.7265625" style="1"/>
+    <col min="6" max="6" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.26953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2852,17 +2876,143 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA7B982-A8FB-2B42-9B70-CF2E4E4052FE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="3" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="36.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="B2" s="3">
+        <v>3953</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.52222222222222225</v>
+      </c>
+      <c r="E2" s="6">
+        <v>43256</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" s="3">
+        <v>9764</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.5229166666666667</v>
+      </c>
+      <c r="E3" s="6">
+        <v>43256</v>
+      </c>
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" s="3">
+        <v>8064</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="E4" s="6">
+        <v>43256</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" s="3">
+        <v>7355</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="E5" s="6">
+        <v>43256</v>
+      </c>
+      <c r="F5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="3">
+        <v>971</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E6" s="6">
+        <v>43256</v>
+      </c>
+      <c r="F6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2991,17 +3141,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0140768B-FC37-6F4D-B32D-F670414C2DE2}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.71875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="10.71875" style="4"/>
+    <col min="1" max="16384" width="10.7265625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
Updated database schema with a FriendsWith table, which shows who is friends with whom. Also commited the updated db.
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="300" yWindow="456" windowWidth="24996" windowHeight="14976" activeTab="2"/>
+    <workbookView xWindow="300" yWindow="456" windowWidth="24996" windowHeight="14976" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="STUDENTS" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="COMMENTS" sheetId="6" r:id="rId3"/>
     <sheet name="CHAIRS" sheetId="5" r:id="rId4"/>
     <sheet name="ATTENDS" sheetId="3" r:id="rId5"/>
+    <sheet name="FRIENDSWITH" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="87">
   <si>
     <t>ID</t>
   </si>
@@ -283,6 +284,12 @@
   </si>
   <si>
     <t>Nah</t>
+  </si>
+  <si>
+    <t>STUDENT_ID1</t>
+  </si>
+  <si>
+    <t>STUDENT_ID2</t>
   </si>
 </sst>
 </file>
@@ -650,7 +657,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="15"/>
@@ -2879,7 +2886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -3373,4 +3380,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3">
+        <v>3953</v>
+      </c>
+      <c r="B2" s="3">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3">
+        <v>8064</v>
+      </c>
+      <c r="B3" s="3">
+        <v>7355</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3">
+        <v>8064</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9764</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated database schema with a Likes table, which shows who likes which comment. Also commited the updated db.
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="300" yWindow="456" windowWidth="24996" windowHeight="14976" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="300" yWindow="456" windowWidth="24996" windowHeight="14976" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="STUDENTS" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="CHAIRS" sheetId="5" r:id="rId4"/>
     <sheet name="ATTENDS" sheetId="3" r:id="rId5"/>
     <sheet name="FRIENDSWITH" sheetId="7" r:id="rId6"/>
+    <sheet name="LIKES" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -290,6 +291,9 @@
   </si>
   <si>
     <t>STUDENT_ID2</t>
+  </si>
+  <si>
+    <t>COMMENT_ID</t>
   </si>
 </sst>
 </file>
@@ -657,7 +661,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="15"/>
@@ -3386,7 +3390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3431,4 +3435,71 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3">
+        <v>7355</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3">
+        <v>971</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3">
+        <v>3953</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3">
+        <v>9764</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3">
+        <v>8064</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>